<commit_message>
"Update DebounceSearchCompany, App, DetailSection, UploadDialog, and BulkTable components; modify state and props; add new route and component"
</commit_message>
<xml_diff>
--- a/public/samplebook.xlsx
+++ b/public/samplebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidde\OneDrive\Desktop\PNQ\cirrusQC\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C664DB-934F-41B7-A58C-A2B2A885FBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F42FDE-6F23-4243-9831-EBF86332F48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -42,13 +42,16 @@
     <t>Link</t>
   </si>
   <si>
-    <t>SocialFeedID</t>
-  </si>
-  <si>
     <t>CompanyID</t>
   </si>
   <si>
     <t>CompanyName</t>
+  </si>
+  <si>
+    <t>https://pnq.co.in/</t>
+  </si>
+  <si>
+    <t>DEMC</t>
   </si>
 </sst>
 </file>
@@ -58,7 +61,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +73,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,10 +124,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -130,8 +142,12 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,39 +426,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" style="4"/>
-    <col min="3" max="3" width="101.5546875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="22" style="3"/>
+    <col min="1" max="1" width="22" style="4"/>
+    <col min="2" max="2" width="101.5546875" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="22" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>35864</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6E8FF2B5-C1C5-4473-BAD4-B52E136E88C0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"Updated various components with new props, state, and functionality; refactored code organization and styling."
</commit_message>
<xml_diff>
--- a/public/samplebook.xlsx
+++ b/public/samplebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidde\OneDrive\Desktop\PNQ\cirrusQC\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F42FDE-6F23-4243-9831-EBF86332F48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13392A85-FAE8-4130-8ED1-C7171AE8E87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -45,13 +45,19 @@
     <t>CompanyID</t>
   </si>
   <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
     <t>https://pnq.co.in/</t>
   </si>
   <si>
     <t>DEMC</t>
+  </si>
+  <si>
+    <t>Headline</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Language</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,29 +445,35 @@
     <col min="3" max="16384" width="22" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>45595</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>35864</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -469,6 +481,6 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{6E8FF2B5-C1C5-4473-BAD4-B52E136E88C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
date format changed in bulk upload
</commit_message>
<xml_diff>
--- a/public/samplebook.xlsx
+++ b/public/samplebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidde\OneDrive\Desktop\PNQ\cirrusQC\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13392A85-FAE8-4130-8ED1-C7171AE8E87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75DE7BA-D921-4A21-98F2-C21733977011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{66010F6D-F8AD-4788-A247-DBA1F160F78D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -45,29 +45,42 @@
     <t>CompanyID</t>
   </si>
   <si>
-    <t>https://pnq.co.in/</t>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Headline</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>https://www.pnq.co.in</t>
   </si>
   <si>
     <t>DEMC</t>
   </si>
   <si>
-    <t>Headline</t>
-  </si>
-  <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>Language</t>
+    <t>Test Headline</t>
+  </si>
+  <si>
+    <t>Test Summary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +97,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -92,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -130,31 +156,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{2BB607B0-76D0-4BF1-8740-4440FCCAD59C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -186,7 +215,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -198,7 +227,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -245,6 +274,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -280,6 +326,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -431,56 +494,397 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284D0A4E-CA49-4570-BC80-DF9412170E62}">
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22" style="4"/>
-    <col min="2" max="2" width="101.5546875" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="22" style="3"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>45598</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>45595</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{6E8FF2B5-C1C5-4473-BAD4-B52E136E88C0}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0DF65FDA-A5F7-473F-8790-AB40E356C59F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>